<commit_message>
Twitter workflow is well named and annotated
</commit_message>
<xml_diff>
--- a/Data/Input/UpdateFile.xlsx
+++ b/Data/Input/UpdateFile.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <x:si>
     <x:t>DATE</x:t>
   </x:si>
@@ -44,7 +44,7 @@
     <x:t>SHOULD_POST_TWITTER</x:t>
   </x:si>
   <x:si>
-    <x:t>05/09/2023</x:t>
+    <x:t>06/09/2023</x:t>
   </x:si>
   <x:si>
     <x:t>Celebrating art-work on Twitter</x:t>
@@ -56,7 +56,7 @@
     <x:t>C:\Users\decadev\Downloads\6.jpg</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> : L-Not Posted : </x:t>
+    <x:t>F-Posted : L-Not Posted : T-Not Posted</x:t>
   </x:si>
   <x:si>
     <x:t>YES</x:t>
@@ -71,7 +71,7 @@
     <x:t>C:\Users\decadev\Downloads\4.jpg</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve"> : L- Posted : </x:t>
+    <x:t>F-Not Posted : L- Posted : T- Posted</x:t>
   </x:si>
   <x:si>
     <x:t>Testing my automation skill</x:t>
@@ -83,10 +83,16 @@
     <x:t>C:\Users\decadev\Downloads\6.jpg;C:\Users\decadev\Downloads\mbappe.jpg;C:\Users\decadev\Downloads\2.jpg</x:t>
   </x:si>
   <x:si>
+    <x:t>F-Posted : L- Posted : T- Posted</x:t>
+  </x:si>
+  <x:si>
     <x:t>I am here</x:t>
   </x:si>
   <x:si>
     <x:t>Project Completed….,!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F-Not Posted : L-Not Posted : T-Not Posted</x:t>
   </x:si>
   <x:si>
     <x:t>NOT DONE</x:t>
@@ -1094,7 +1100,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:H11"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <x:selection activeCell="E2" sqref="E2 E2:E5"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1199,7 +1205,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="E4" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
         <x:v>13</x:v>
@@ -1216,13 +1222,13 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E5" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
         <x:v>14</x:v>
@@ -1312,7 +1318,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:5">
       <x:c r="E2" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Time trigger added in the orchestrator together with some corrections in the code
</commit_message>
<xml_diff>
--- a/Data/Input/UpdateFile.xlsx
+++ b/Data/Input/UpdateFile.xlsx
@@ -44,7 +44,7 @@
     <x:t>SHOULD_POST_TWITTER</x:t>
   </x:si>
   <x:si>
-    <x:t>06/09/2023</x:t>
+    <x:t>07/09/2023</x:t>
   </x:si>
   <x:si>
     <x:t>Celebrating art-work on Twitter</x:t>
@@ -53,10 +53,10 @@
     <x:t>Hello People, rounding up with the project.,..!</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Users\decadev\Downloads\6.jpg</x:t>
-  </x:si>
-  <x:si>
-    <x:t>F-Posted : L-Not Posted : T-Not Posted</x:t>
+    <x:t>C:\Users\decadev\Downloads\2.jpg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>F-Posted : L-Not Posted : T- Posted</x:t>
   </x:si>
   <x:si>
     <x:t>YES</x:t>
@@ -80,7 +80,7 @@
     <x:t>This is me testing my automation</x:t>
   </x:si>
   <x:si>
-    <x:t>C:\Users\decadev\Downloads\6.jpg;C:\Users\decadev\Downloads\mbappe.jpg;C:\Users\decadev\Downloads\2.jpg</x:t>
+    <x:t>C:\Users\decadev\Downloads\3.jpg;C:\Users\decadev\Downloads\mbappe.jpg;C:\Users\decadev\Downloads\2.jpg</x:t>
   </x:si>
   <x:si>
     <x:t>F-Posted : L- Posted : T- Posted</x:t>
@@ -1098,10 +1098,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H11"/>
+  <x:dimension ref="A1:H20"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2 E2:E5"/>
+    <x:sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <x:selection activeCell="E2" sqref="E2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="255" defaultRowHeight="14.4"/>
@@ -1245,12 +1245,16 @@
     </x:row>
     <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s"/>
+      <x:c r="D8" s="0" t="s"/>
     </x:row>
     <x:row r="9" spans="1:8">
       <x:c r="D9" s="0" t="s"/>
     </x:row>
     <x:row r="11" spans="1:8">
       <x:c r="A11" s="0" t="s"/>
+    </x:row>
+    <x:row r="20" spans="1:8">
+      <x:c r="A20" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>